<commit_message>
addition of eswatini cause of death profile
</commit_message>
<xml_diff>
--- a/observations-summary.xlsx
+++ b/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Profile</t>
   </si>
@@ -47,16 +47,43 @@
     <t>Method</t>
   </si>
   <si>
+    <t>SzCauseOfDeath</t>
+  </si>
+  <si>
+    <t>Eswatini Cause of Death Profile</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>LOINC#79378-6</t>
+  </si>
+  <si>
+    <t>dateTime, Period, Timing, instant</t>
+  </si>
+  <si>
+    <t>CodeableConcept</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>LOINC#69440-6</t>
+  </si>
+  <si>
+    <t>Quantity, CodeableConcept, string</t>
+  </si>
+  <si>
     <t>SzVitalSigns</t>
   </si>
   <si>
     <t>Eswatini Vital Signs Profile</t>
   </si>
   <si>
-    <t>null#vital-signs</t>
-  </si>
-  <si>
-    <t/>
+    <t>Observation Category Codes#vital-signs</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/observation-vitalsignresult (required)</t>
@@ -66,9 +93,6 @@
   </si>
   <si>
     <t>Quantityĵ</t>
-  </si>
-  <si>
-    <t>optional</t>
   </si>
 </sst>
 </file>
@@ -202,7 +226,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -254,28 +278,133 @@
         <v>13</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s" s="2">
         <v>14</v>
       </c>
       <c r="F2" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="H2" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="H2" t="s" s="2">
+      <c r="I2" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="I2" t="s" s="2">
+      <c r="J2" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="J2" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s" s="2">
-        <v>14</v>
+      <c r="I3" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s" s="2">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>